<commit_message>
Homework, minor and major updates
</commit_message>
<xml_diff>
--- a/public/downloads/beneficiary-account-import-template.xlsx
+++ b/public/downloads/beneficiary-account-import-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jevohngentry/Desktop/invictus/public/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6520D3B2-0937-474E-BE43-FEDCA3870038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5E66E-7F69-7F48-B310-8FF4494E2E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="3620" windowWidth="27640" windowHeight="16940" xr2:uid="{BAD56F22-FF8B-294C-89A7-6D7F690EC2C2}"/>
+    <workbookView xWindow="4380" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{BAD56F22-FF8B-294C-89A7-6D7F690EC2C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Client ID*</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Account Number*</t>
   </si>
   <si>
-    <t>Primary Beneficiary Name (Last, First)</t>
-  </si>
-  <si>
-    <t>Primary Beneficiary Relationship</t>
-  </si>
-  <si>
-    <t>Primary Beneficiary Allocation (%)</t>
-  </si>
-  <si>
-    <t>Contingent Beneficiary Name (Last, First)</t>
-  </si>
-  <si>
-    <t>Contingent Beneficiary Relationship</t>
-  </si>
-  <si>
-    <t>Contingent Beneficiary Allocation (%)</t>
+    <t>Beneficiary Name (Last, First)</t>
+  </si>
+  <si>
+    <t>Beneficiary Type (Primary / Contingent)</t>
+  </si>
+  <si>
+    <t>Beneficiary Allocation (%)</t>
+  </si>
+  <si>
+    <t>Beneficiary Relationship (Spouse, Child, etc.)</t>
+  </si>
+  <si>
+    <t>Client ID</t>
   </si>
 </sst>
 </file>
@@ -449,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0773A9-000A-C142-9AC0-9D9174053A82}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,28 +460,22 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="K1" s="2"/>
     </row>

</xml_diff>